<commit_message>
Makes variable names unique for reporting
</commit_message>
<xml_diff>
--- a/projects/ptool_small_full_factorial_measures.xlsx
+++ b/projects/ptool_small_full_factorial_measures.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="802">
   <si>
     <t>type</t>
   </si>
@@ -2292,9 +2292,6 @@
     <t>Add EIFS Wall Insulation</t>
   </si>
   <si>
-    <t>Apply Measure</t>
-  </si>
-  <si>
     <t>apply_measure</t>
   </si>
   <si>
@@ -2434,6 +2431,21 @@
   </si>
   <si>
     <t>Sunday End Time</t>
+  </si>
+  <si>
+    <t>Apply EIFS Wall Insulation</t>
+  </si>
+  <si>
+    <t>Apply Wireless Lighting Occupancy Sensors</t>
+  </si>
+  <si>
+    <t>Apply Energy Recovery Ventilator</t>
+  </si>
+  <si>
+    <t>Apply Add Demand Control Ventilation</t>
+  </si>
+  <si>
+    <t>Apply Advanced Power Strips</t>
   </si>
 </sst>
 </file>
@@ -6105,7 +6117,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6517,7 +6529,7 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6818,10 +6830,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>797</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>750</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>751</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>61</v>
@@ -6830,7 +6842,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="K9" s="23" t="b">
         <v>1</v>
@@ -6842,7 +6854,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R9" s="44" t="s">
         <v>723</v>
@@ -6853,10 +6865,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>63</v>
@@ -6880,13 +6892,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="43" t="s">
+        <v>755</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>757</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>756</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>758</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>757</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>67</v>
@@ -6897,10 +6909,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="23" t="s">
+        <v>798</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>750</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>751</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>61</v>
@@ -6909,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="K12" s="23" t="b">
         <v>1</v>
@@ -6921,7 +6933,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R12" s="44" t="s">
         <v>723</v>
@@ -6932,10 +6944,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G13" s="32" t="s">
         <v>63</v>
@@ -6959,13 +6971,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E14" s="43" t="s">
         <v>67</v>
@@ -6976,10 +6988,10 @@
         <v>22</v>
       </c>
       <c r="D15" s="23" t="s">
+        <v>799</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>750</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>751</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>61</v>
@@ -6988,7 +7000,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="K15" s="23" t="b">
         <v>1</v>
@@ -7000,7 +7012,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R15" s="44" t="s">
         <v>723</v>
@@ -7011,10 +7023,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G16" s="32" t="s">
         <v>63</v>
@@ -7038,10 +7050,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G17" s="32" t="s">
         <v>63</v>
@@ -7065,10 +7077,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="45" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G18" s="32" t="s">
         <v>63</v>
@@ -7092,10 +7104,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G19" s="32" t="s">
         <v>63</v>
@@ -7119,10 +7131,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G20" s="32" t="s">
         <v>63</v>
@@ -7146,10 +7158,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G21" s="32" t="s">
         <v>63</v>
@@ -7173,10 +7185,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G22" s="32" t="s">
         <v>63</v>
@@ -7200,10 +7212,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="45" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G23" s="32" t="s">
         <v>63</v>
@@ -7227,10 +7239,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="45" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>63</v>
@@ -7254,13 +7266,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="43" t="s">
+        <v>782</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>783</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>784</v>
-      </c>
       <c r="D25" s="43" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E25" s="43" t="s">
         <v>67</v>
@@ -7271,10 +7283,10 @@
         <v>22</v>
       </c>
       <c r="D26" s="23" t="s">
+        <v>800</v>
+      </c>
+      <c r="E26" s="23" t="s">
         <v>750</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>751</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>61</v>
@@ -7283,7 +7295,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="K26" s="23" t="b">
         <v>1</v>
@@ -7295,7 +7307,7 @@
         <v>1</v>
       </c>
       <c r="P26" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R26" s="44" t="s">
         <v>723</v>
@@ -7306,13 +7318,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="43" t="s">
+        <v>785</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>784</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>786</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>785</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>787</v>
       </c>
       <c r="E27" s="43" t="s">
         <v>67</v>
@@ -7323,10 +7335,10 @@
         <v>22</v>
       </c>
       <c r="D28" s="23" t="s">
+        <v>801</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>750</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>751</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>61</v>
@@ -7335,7 +7347,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="K28" s="23" t="b">
         <v>1</v>
@@ -7347,7 +7359,7 @@
         <v>1</v>
       </c>
       <c r="P28" s="23" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="R28" s="44" t="s">
         <v>723</v>
@@ -7358,7 +7370,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="45" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>297</v>
@@ -7385,7 +7397,7 @@
         <v>21</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>299</v>
@@ -7412,7 +7424,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="45" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>301</v>
@@ -7439,7 +7451,7 @@
         <v>21</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>303</v>
@@ -7466,7 +7478,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>305</v>
@@ -7493,7 +7505,7 @@
         <v>21</v>
       </c>
       <c r="D34" s="45" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>307</v>
@@ -7520,7 +7532,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="45" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E35" s="33" t="s">
         <v>309</v>
@@ -7547,7 +7559,7 @@
         <v>21</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>311</v>
@@ -7574,7 +7586,7 @@
         <v>21</v>
       </c>
       <c r="D37" s="45" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>313</v>
@@ -7601,7 +7613,7 @@
         <v>21</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
update to most recent version of openstudio analysisl
</commit_message>
<xml_diff>
--- a/projects/ptool_small_full_factorial_measures.xlsx
+++ b/projects/ptool_small_full_factorial_measures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="33600" windowHeight="19840" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -5964,8 +5964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6070,7 +6070,7 @@
         <v>442</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>439</v>
+        <v>603</v>
       </c>
       <c r="C8" s="36" t="str">
         <f>VLOOKUP($B8,instance_defs,5,FALSE)</f>
@@ -6078,11 +6078,11 @@
       </c>
       <c r="D8" s="36" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v>8 Cores with 80 GB</v>
+        <v>32 Cores with 320 GB</v>
       </c>
       <c r="E8" s="36" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$0.42/hour</v>
+        <v>$1.68/hour</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>443</v>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="E9" s="36" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$0.7/hour</v>
+        <v>$1.96/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>606</v>
@@ -6547,7 +6547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>